<commit_message>
Add minor, major conflcits in the ga, update the display function to show them
</commit_message>
<xml_diff>
--- a/data/Course list and attributes.xlsx
+++ b/data/Course list and attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/zuh11_psu_edu/Documents/Scheduler project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F71A95F8-7CCC-4C0E-A364-FC8ACE03AD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB8468AE-9A5E-4BF2-A29B-F00A1D7B99E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="460" windowWidth="13680" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20780" yWindow="460" windowWidth="13680" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S&amp;E Courses" sheetId="1" r:id="rId1"/>
@@ -2226,9 +2226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15"/>
@@ -5630,7 +5630,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A4" sqref="A4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6563,13 +6563,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F66A28-76E8-4CD3-989A-696474DCFCEC}">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
@@ -7023,7 +7023,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>